<commit_message>
496680 Added comment to US114 - moved to Build 2
</commit_message>
<xml_diff>
--- a/Requirement/eBilling Build 1 IB_2_576 Epic Sub Epic Story Links.xlsx
+++ b/Requirement/eBilling Build 1 IB_2_576 Epic Sub Epic Story Links.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Story ID</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Build 1 IB*2*576</t>
+  </si>
+  <si>
+    <t>MOVED TO BUILD 2</t>
   </si>
 </sst>
 </file>
@@ -279,7 +282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -314,6 +317,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -323,11 +332,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -634,7 +640,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,14 +656,14 @@
       <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="16"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18"/>
       <c r="F1" s="1"/>
       <c r="G1"/>
     </row>
@@ -665,7 +671,7 @@
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="15" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -714,7 +720,9 @@
       <c r="E4" s="9">
         <v>464021</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="19" t="s">
+        <v>18</v>
+      </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
496680 Uploaded FInal Version
</commit_message>
<xml_diff>
--- a/Requirement/eBilling Build 1 IB_2_576 Epic Sub Epic Story Links.xlsx
+++ b/Requirement/eBilling Build 1 IB_2_576 Epic Sub Epic Story Links.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Story ID</t>
   </si>
@@ -66,13 +66,16 @@
     <t>Sub Epic ID</t>
   </si>
   <si>
-    <t>US ID</t>
-  </si>
-  <si>
     <t>Build 1 IB*2*576</t>
   </si>
   <si>
     <t>MOVED TO BUILD 2</t>
+  </si>
+  <si>
+    <t>US ID (RTC)</t>
+  </si>
+  <si>
+    <t>US ID (RM)</t>
   </si>
 </sst>
 </file>
@@ -282,7 +285,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -311,9 +314,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -321,19 +321,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -637,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,29 +655,32 @@
     <col min="2" max="2" width="50.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" style="3" customWidth="1"/>
     <col min="4" max="4" width="11.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="3"/>
+    <col min="5" max="5" width="13" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>17</v>
+      <c r="B1" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D1" s="17"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="1"/>
-      <c r="G1"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="1"/>
+      <c r="H1"/>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -681,129 +690,148 @@
         <v>15</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="8">
-        <v>811607</v>
+        <v>888501</v>
       </c>
       <c r="D3" s="8">
-        <v>820292</v>
-      </c>
-      <c r="E3" s="9">
+        <v>888528</v>
+      </c>
+      <c r="E3" s="19">
+        <v>891594</v>
+      </c>
+      <c r="F3" s="9">
         <v>464014</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="8">
-        <v>811607</v>
+        <v>888501</v>
       </c>
       <c r="D4" s="8">
-        <v>874429</v>
-      </c>
-      <c r="E4" s="9">
+        <v>888528</v>
+      </c>
+      <c r="E4" s="19">
+        <v>891595</v>
+      </c>
+      <c r="F4" s="9">
         <v>464021</v>
       </c>
-      <c r="F4" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="8">
-        <v>811607</v>
+        <v>888501</v>
       </c>
       <c r="D5" s="8">
-        <v>828589</v>
-      </c>
-      <c r="E5" s="9">
+        <v>888528</v>
+      </c>
+      <c r="E5" s="19">
+        <v>891601</v>
+      </c>
+      <c r="F5" s="9">
         <v>464354</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="3"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="8">
-        <v>811607</v>
+        <v>888501</v>
       </c>
       <c r="D6" s="8">
-        <v>828587</v>
-      </c>
-      <c r="E6" s="9">
+        <v>888528</v>
+      </c>
+      <c r="E6" s="19">
+        <v>891621</v>
+      </c>
+      <c r="F6" s="9">
         <v>464374</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="8">
-        <v>811607</v>
+        <v>888503</v>
       </c>
       <c r="D7" s="8">
-        <v>828598</v>
-      </c>
-      <c r="E7" s="9">
+        <v>888545</v>
+      </c>
+      <c r="E7" s="19">
+        <v>891624</v>
+      </c>
+      <c r="F7" s="9">
         <v>464398</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="3"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C1:F1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" location="action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_HFthQYQREeahi_YbqnplZQ&amp;linkURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Flinks%2F_BnrG84qCEea1ifQx2pA2" display="811607"/>
-    <hyperlink ref="C6" r:id="rId2" location="action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_HFthQYQREeahi_YbqnplZQ&amp;linkURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Flinks%2F_BnrG84qCEea1ifQx2pA2" display="811607"/>
-    <hyperlink ref="C7" r:id="rId3" location="action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_HFthQYQREeahi_YbqnplZQ&amp;linkURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Flinks%2F_BnrG84qCEea1ifQx2pA2" display="811607"/>
-    <hyperlink ref="C3" r:id="rId4" location="action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_HFthQYQREeahi_YbqnplZQ&amp;linkURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Flinks%2F_BnrG84qCEea1ifQx2pA2" display="811607"/>
-    <hyperlink ref="C4" r:id="rId5" location="action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_HFthQYQREeahi_YbqnplZQ&amp;linkURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Flinks%2F_BnrG84qCEea1ifQx2pA2" display="811607"/>
-    <hyperlink ref="E6" r:id="rId6" location="action=com.ibm.team.workitem.viewWorkItem&amp;id=464374&amp;tab=com.ibm.team.workitem.tab.links" display="https://clm.rational.oit.va.gov/ccm/web/projects/MCCF_EDI_TAS (CM) - action=com.ibm.team.workitem.viewWorkItem&amp;id=464374&amp;tab=com.ibm.team.workitem.tab.links"/>
-    <hyperlink ref="E7" r:id="rId7" location="action=com.ibm.team.workitem.viewWorkItem&amp;id=464398" display="https://clm.rational.oit.va.gov/ccm/web/projects/MCCF_EDI_TAS (CM) - action=com.ibm.team.workitem.viewWorkItem&amp;id=464398"/>
-    <hyperlink ref="E5" r:id="rId8" location="action=com.ibm.team.workitem.viewWorkItem&amp;id=464354" display="https://clm.rational.oit.va.gov/ccm/web/projects/MCCF_EDI_TAS (CM) - action=com.ibm.team.workitem.viewWorkItem&amp;id=464354"/>
-    <hyperlink ref="E4" r:id="rId9" location="action=com.ibm.team.workitem.viewWorkItem&amp;id=464021" display="https://clm.rational.oit.va.gov/ccm/web/projects/MCCF_EDI_TAS (CM) - action=com.ibm.team.workitem.viewWorkItem&amp;id=464021"/>
-    <hyperlink ref="E3" r:id="rId10" location="action=com.ibm.team.workitem.viewWorkItem&amp;id=464014" display="https://clm.rational.oit.va.gov/ccm/web/projects/MCCF_EDI_TAS (CM) - action=com.ibm.team.workitem.viewWorkItem&amp;id=464014"/>
-    <hyperlink ref="D3" r:id="rId11" location="action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_dq3uM4TrEeahi_YbqnplZQ&amp;vvc.configuration=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fcm%2Fstream%2F_WI1K" display="https://clm.rational.oit.va.gov/rm/web - action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_dq3uM4TrEeahi_YbqnplZQ&amp;vvc.configuration=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fcm%2Fstream%2F_WI1K"/>
-    <hyperlink ref="D6" r:id="rId12" location="action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_7xc-dYzGEea1ifQx2pA2Fg&amp;linkURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Flinks%2F_DpErQZR4Eeays8wDvf3-" display="https://clm.rational.oit.va.gov/rm/web - action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_7xc-dYzGEea1ifQx2pA2Fg&amp;linkURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Flinks%2F_DpErQZR4Eeays8wDvf3-"/>
-    <hyperlink ref="D7" r:id="rId13" location="action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_7xKDh4zGEea1ifQx2pA2Fg&amp;vvc.configuration=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fcm%2Fstream%2F_WI1K" display="https://clm.rational.oit.va.gov/rm/web - action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_7xKDh4zGEea1ifQx2pA2Fg&amp;vvc.configuration=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fcm%2Fstream%2F_WI1K"/>
-    <hyperlink ref="D5" r:id="rId14" location="action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_7wHhs4zGEea1ifQx2pA2Fg&amp;vvc.configuration=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fcm%2Fstream%2F_WI1K" display="https://clm.rational.oit.va.gov/rm/web - action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_7wHhs4zGEea1ifQx2pA2Fg&amp;vvc.configuration=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fcm%2Fstream%2F_WI1K"/>
-    <hyperlink ref="D4" r:id="rId15" location="action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_bBrOsfIVEeaE34UfLhff7w&amp;vvc.configuration=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fcm%2Fstream%2F_WI1K" display="https://clm.rational.oit.va.gov/rm/web - action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_bBrOsfIVEeaE34UfLhff7w&amp;vvc.configuration=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fcm%2Fstream%2F_WI1K"/>
+    <hyperlink ref="F6" r:id="rId1" location="action=com.ibm.team.workitem.viewWorkItem&amp;id=464374&amp;tab=com.ibm.team.workitem.tab.links" display="https://clm.rational.oit.va.gov/ccm/web/projects/MCCF_EDI_TAS (CM) - action=com.ibm.team.workitem.viewWorkItem&amp;id=464374&amp;tab=com.ibm.team.workitem.tab.links"/>
+    <hyperlink ref="F7" r:id="rId2" location="action=com.ibm.team.workitem.viewWorkItem&amp;id=464398" display="https://clm.rational.oit.va.gov/ccm/web/projects/MCCF_EDI_TAS (CM) - action=com.ibm.team.workitem.viewWorkItem&amp;id=464398"/>
+    <hyperlink ref="F5" r:id="rId3" location="action=com.ibm.team.workitem.viewWorkItem&amp;id=464354" display="https://clm.rational.oit.va.gov/ccm/web/projects/MCCF_EDI_TAS (CM) - action=com.ibm.team.workitem.viewWorkItem&amp;id=464354"/>
+    <hyperlink ref="F4" r:id="rId4" location="action=com.ibm.team.workitem.viewWorkItem&amp;id=464021" display="https://clm.rational.oit.va.gov/ccm/web/projects/MCCF_EDI_TAS (CM) - action=com.ibm.team.workitem.viewWorkItem&amp;id=464021"/>
+    <hyperlink ref="F3" r:id="rId5" location="action=com.ibm.team.workitem.viewWorkItem&amp;id=464014" display="https://clm.rational.oit.va.gov/ccm/web/projects/MCCF_EDI_TAS (CM) - action=com.ibm.team.workitem.viewWorkItem&amp;id=464014"/>
+    <hyperlink ref="E3" r:id="rId6" location="action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_nrAtgSX5EeeMa7rbcelMLw&amp;editMode=true&amp;vvc.configuration=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fcm%2Fstream%2F_WI1KgHnyEea6E-3s3yro6A" display="https://clm.rational.oit.va.gov/rm/web - action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_nrAtgSX5EeeMa7rbcelMLw&amp;editMode=true&amp;vvc.configuration=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fcm%2Fstream%2F_WI1KgHnyEea6E-3s3yro6A"/>
+    <hyperlink ref="D3" r:id="rId7" location="action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_yRAD8R4mEeepL52rEMDxQw&amp;linkURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Flinks%2F_zQMn8yX5EeeMa7rbcelMLw&amp;vvc.configuration=https%3A%2F%2Fclm" display="https://clm.rational.oit.va.gov/rm/web - action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_yRAD8R4mEeepL52rEMDxQw&amp;linkURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Flinks%2F_zQMn8yX5EeeMa7rbcelMLw&amp;vvc.configuration=https%3A%2F%2Fclm"/>
+    <hyperlink ref="C3" r:id="rId8" location="action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_yRY3wR4hEeepL52rEMDxQw&amp;linkURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Flinks%2F_9h1pkx4nEeepL52rEMDx" display="https://clm.rational.oit.va.gov/rm/web - action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_yRY3wR4hEeepL52rEMDxQw&amp;linkURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Flinks%2F_9h1pkx4nEeepL52rEMDx"/>
+    <hyperlink ref="D4:D6" r:id="rId9" location="action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_yRAD8R4mEeepL52rEMDxQw&amp;linkURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Flinks%2F_zQMn8yX5EeeMa7rbcelMLw&amp;vvc.configuration=https%3A%2F%2Fclm" display="https://clm.rational.oit.va.gov/rm/web - action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_yRAD8R4mEeepL52rEMDxQw&amp;linkURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Flinks%2F_zQMn8yX5EeeMa7rbcelMLw&amp;vvc.configuration=https%3A%2F%2Fclm"/>
+    <hyperlink ref="C4:C6" r:id="rId10" location="action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_yRY3wR4hEeepL52rEMDxQw&amp;linkURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Flinks%2F_9h1pkx4nEeepL52rEMDx" display="https://clm.rational.oit.va.gov/rm/web - action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_yRY3wR4hEeepL52rEMDxQw&amp;linkURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Flinks%2F_9h1pkx4nEeepL52rEMDx"/>
+    <hyperlink ref="E4" r:id="rId11" location="action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_iZiXYSX6EeeMa7rbcelMLw&amp;editMode=true&amp;vvc.configuration=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fcm%2F" display="https://clm.rational.oit.va.gov/rm/web - action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_iZiXYSX6EeeMa7rbcelMLw&amp;editMode=true&amp;vvc.configuration=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fcm%2F"/>
+    <hyperlink ref="E5" r:id="rId12" location="action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_fxJ4gSX9EeeMa7rbcelMLw&amp;editMode=true&amp;vvc.configuration=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fcm%2F" display="https://clm.rational.oit.va.gov/rm/web - action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_fxJ4gSX9EeeMa7rbcelMLw&amp;editMode=true&amp;vvc.configuration=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fcm%2F"/>
+    <hyperlink ref="E6" r:id="rId13" location="action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_x-1fASX_EeeMa7rbcelMLw&amp;editMode=true&amp;vvc.configuration=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fcm%2Fstream%2F_WI1KgHnyEea6E-3s3yro6A" display="https://clm.rational.oit.va.gov/rm/web - action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_x-1fASX_EeeMa7rbcelMLw&amp;editMode=true&amp;vvc.configuration=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fcm%2Fstream%2F_WI1KgHnyEea6E-3s3yro6A"/>
+    <hyperlink ref="E7" r:id="rId14" location="action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_nxTelyYAEeeMa7rbcelMLw&amp;editMode=true&amp;vvc.configuration=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fcm%2F" display="https://clm.rational.oit.va.gov/rm/web - action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_nxTelyYAEeeMa7rbcelMLw&amp;editMode=true&amp;vvc.configuration=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fcm%2F"/>
+    <hyperlink ref="D7" r:id="rId15" location="action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_13S4Yx4qEeepL52rEMDxQw&amp;linkURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Flinks%2F_vv00UyYAEeeMa7rbcelMLw&amp;vvc.configuration=https%3A%2F%2Fclm" display="https://clm.rational.oit.va.gov/rm/web - action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_13S4Yx4qEeepL52rEMDxQw&amp;linkURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Flinks%2F_vv00UyYAEeeMa7rbcelMLw&amp;vvc.configuration=https%3A%2F%2Fclm"/>
+    <hyperlink ref="C7" r:id="rId16" location="action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_Tt0yUR4iEeepL52rEMDxQw&amp;linkURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Flinks%2F_Crx3gR4rEeepL52rEMDx" display="https://clm.rational.oit.va.gov/rm/web - action=com.ibm.rdm.web.pages.showArtifact&amp;artifactURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Fresources%2F_Tt0yUR4iEeepL52rEMDxQw&amp;linkURI=https%3A%2F%2Fclm.rational.oit.va.gov%2Frm%2Flinks%2F_Crx3gR4rEeepL52rEMDx"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 

</xml_diff>